<commit_message>
update images and link matrix
</commit_message>
<xml_diff>
--- a/Deliverables/Traceability Link Matrix.xlsx
+++ b/Deliverables/Traceability Link Matrix.xlsx
@@ -1,18 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brittanynall/Documents/GitHub/cs414-f18-801-CtrlAltDefeat/Deliverables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - Traceability Link Mat" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - Traceability Link Mat" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="40">
   <si>
     <t>Traceability Link Matrix - Team CtrlAltDefeat - Brittany Nall &amp; Melissa Smith</t>
   </si>
@@ -120,16 +135,25 @@
   </si>
   <si>
     <t>UC - 19</t>
+  </si>
+  <si>
+    <t>GymSystemCreator</t>
+  </si>
+  <si>
+    <t>GymSystemController</t>
+  </si>
+  <si>
+    <t>SystemDao</t>
+  </si>
+  <si>
+    <t>Response</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -141,7 +165,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -282,81 +306,137 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="14">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -555,7 +635,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -574,7 +654,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -604,7 +684,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -630,7 +710,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -656,7 +736,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -682,7 +762,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -708,7 +788,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -734,7 +814,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -760,7 +840,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -786,7 +866,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +892,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,9 +905,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -844,7 +930,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -863,7 +949,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -889,7 +975,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -915,7 +1001,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -941,7 +1027,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -967,7 +1053,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -993,7 +1079,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1019,7 +1105,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1045,7 +1131,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1071,7 +1157,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1097,7 +1183,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1110,9 +1196,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1126,7 +1218,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1145,7 +1237,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1175,7 +1267,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1201,7 +1293,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1227,7 +1319,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1253,7 +1345,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1279,7 +1371,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1305,7 +1397,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1331,7 +1423,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1357,7 +1449,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1383,7 +1475,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1396,592 +1488,806 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:P21"/>
+  <dimension ref="A1:IV21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight" activeCell="U15" sqref="U15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5547" style="1" customWidth="1"/>
-    <col min="9" max="9" width="18.1484" style="1" customWidth="1"/>
-    <col min="10" max="16" width="16.3516" style="1" customWidth="1"/>
-    <col min="17" max="256" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="7" width="16.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.1640625" style="1" customWidth="1"/>
+    <col min="10" max="16" width="16.33203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.33203125" style="1" customWidth="1"/>
+    <col min="19" max="256" width="16.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:20" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" t="s" s="4">
+    <row r="2" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="4">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="4">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s" s="4">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s" s="4">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G2" t="s" s="4">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s" s="4">
+      <c r="H2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I2" t="s" s="4">
+      <c r="I2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J2" t="s" s="4">
+      <c r="J2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K2" t="s" s="4">
+      <c r="K2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" t="s" s="4">
+      <c r="L2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" t="s" s="4">
+      <c r="M2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" t="s" s="4">
+      <c r="N2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O2" t="s" s="4">
+      <c r="O2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P2" t="s" s="4">
+      <c r="P2" s="3" t="s">
         <v>15</v>
       </c>
+      <c r="Q2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="5">
+    <row r="3" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="J3" s="7"/>
-      <c r="K3" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="L3" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s" s="8">
-        <v>17</v>
-      </c>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="7"/>
+      <c r="B3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="9">
+    <row r="4" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B4" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="I4" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
+      <c r="B4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="R4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="9">
+    <row r="5" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="9">
+    <row r="6" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="J6" s="12"/>
-      <c r="K6" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="L6" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M6" s="12"/>
-      <c r="N6" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="O6" s="12"/>
-      <c r="P6" t="s" s="11">
+      <c r="B6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="11"/>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="11"/>
+      <c r="K6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M6" s="11"/>
+      <c r="N6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="11"/>
+      <c r="P6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T6" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="9">
+    <row r="7" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
+      <c r="B7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" t="s" s="9">
+    <row r="8" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" t="s" s="9">
+    <row r="9" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="J9" s="12"/>
-      <c r="K9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="L9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M9" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="11"/>
+      <c r="K9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" t="s" s="9">
+    <row r="10" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T10" s="11"/>
     </row>
-    <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" t="s" s="9">
+    <row r="11" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T11" s="11"/>
     </row>
-    <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" t="s" s="9">
+    <row r="12" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="12"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T12" s="11"/>
     </row>
-    <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" t="s" s="9">
+    <row r="13" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="12"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="11"/>
+      <c r="R13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S13" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T13" s="10"/>
     </row>
-    <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" t="s" s="9">
+    <row r="14" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="P14" s="12"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="R14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S14" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T14" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" t="s" s="9">
+    <row r="15" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="P15" s="12"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S15" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T15" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" t="s" s="9">
+    <row r="16" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="P16" s="12"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T16" s="11"/>
     </row>
-    <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" t="s" s="9">
+    <row r="17" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="P17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T17" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" t="s" s="9">
+    <row r="18" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="12"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="P18" s="12"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T18" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" t="s" s="9">
+    <row r="19" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B19" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C19" s="12"/>
-      <c r="D19" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
+      <c r="B19" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="R19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T19" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" t="s" s="9">
+    <row r="20" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s" s="10">
-        <v>17</v>
-      </c>
-      <c r="C20" s="12"/>
-      <c r="D20" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="H20" s="12"/>
-      <c r="I20" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="J20" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="K20" s="12"/>
-      <c r="L20" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="12"/>
+      <c r="B20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T20" s="10" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" t="s" s="9">
+    <row r="21" spans="1:20" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="12"/>
-      <c r="D21" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" t="s" s="11">
-        <v>17</v>
-      </c>
-      <c r="H21" s="12"/>
-      <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="12"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="T21" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:P1"/>
   </mergeCells>
-  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>